<commit_message>
Revert "Revert "new excel""
This reverts commit 577eb7286cb3fae44296d8b090ad8ff80b3142fe.
</commit_message>
<xml_diff>
--- a/target/classes/testdata/reg.xlsx
+++ b/target/classes/testdata/reg.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="293" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="293" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Reg" sheetId="1" state="visible" r:id="rId2"/>
@@ -157,19 +157,19 @@
     <t>Tagasiside</t>
   </si>
   <si>
-    <t>tavalinetont31</t>
+    <t>tavalinetont33</t>
   </si>
   <si>
     <t>Toivo Tavaline</t>
   </si>
   <si>
-    <t>puhtaloom31</t>
+    <t>puhtaloom33</t>
   </si>
   <si>
     <t>Martin Loom</t>
   </si>
   <si>
-    <t>filmweird31</t>
+    <t>filmweird33</t>
   </si>
   <si>
     <t>Toomas Film</t>
@@ -208,13 +208,13 @@
     <t>Oma küla vana</t>
   </si>
   <si>
-    <t>Jalgpalliäss</t>
+    <t>Jalgpalliass</t>
   </si>
   <si>
     <t>Eks sa tea paremini</t>
   </si>
   <si>
-    <t>selentest16@mailinator.com</t>
+    <t>selentest20@mailinator.com</t>
   </si>
   <si>
     <t>selentest@hotmail.com</t>
@@ -232,7 +232,7 @@
     <t>Eks kaitsetöö ole kah tähtis</t>
   </si>
   <si>
-    <t>testimeauto13@mailinator.com</t>
+    <t>testimeauto20@mailinator.com</t>
   </si>
   <si>
     <t>Sa ei tea kes ma olen</t>
@@ -247,7 +247,7 @@
     <t>Indeed</t>
   </si>
   <si>
-    <t>vahekonto11@mailinator.com</t>
+    <t>vahekonto20@mailinator.com</t>
   </si>
   <si>
     <t>Password</t>
@@ -289,10 +289,10 @@
     <t>Tavaline</t>
   </si>
   <si>
-    <t>Kas see on tavaline küsitlius</t>
-  </si>
-  <si>
-    <t>Tundub täiesti tavaline</t>
+    <t>Kas see on tavaline kysitlus</t>
+  </si>
+  <si>
+    <t>Tundub taiesti tavaline</t>
   </si>
   <si>
     <t>Mis meeldib mulle</t>
@@ -307,7 +307,7 @@
     <t>Draama</t>
   </si>
   <si>
-    <t>Õnnenumbrid on mul</t>
+    <t>6nnenumbrid on mul</t>
   </si>
   <si>
     <t>Kolmteist</t>
@@ -316,7 +316,7 @@
     <t>Seitse</t>
   </si>
   <si>
-    <t>Üks</t>
+    <t>Yks</t>
   </si>
   <si>
     <t>Loomaed</t>
@@ -355,10 +355,10 @@
     <t>Filmid</t>
   </si>
   <si>
-    <t>Kas liiga palju järge on halb?</t>
-  </si>
-  <si>
-    <t>Kahjuks küll, kuid raha toovad nad sisse</t>
+    <t>Kas liiga palju jarge on halb?</t>
+  </si>
+  <si>
+    <t>Ei, kuid ju siis toovad raha sisse</t>
   </si>
   <si>
     <t>Minu lemmikfilmi zanr</t>
@@ -424,7 +424,7 @@
     <t>Sinu jaoks jah</t>
   </si>
   <si>
-    <t>Väravaid oskab lüüa, kuid kaitsa ei oska</t>
+    <t>Väravaid oskab lyya, kuid kaitsa ei oska</t>
   </si>
   <si>
     <t>Eks me kõik oleme natuke imelikud</t>
@@ -818,7 +818,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet4!A2</f>
-        <v>tavalinetont31</v>
+        <v>tavalinetont33</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">Sheet6!B2</f>
@@ -835,7 +835,7 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet4!C2</f>
-        <v>puhtaloom31</v>
+        <v>puhtaloom33</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">Sheet6!B3</f>
@@ -852,7 +852,7 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet4!E2</f>
-        <v>filmweird31</v>
+        <v>filmweird33</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">Sheet6!B4</f>
@@ -908,7 +908,7 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet2!A2</f>
-        <v>tavalinetont31</v>
+        <v>tavalinetont33</v>
       </c>
       <c r="B2" s="2" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -921,7 +921,7 @@
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet2!A3</f>
-        <v>puhtaloom31</v>
+        <v>puhtaloom33</v>
       </c>
       <c r="B3" s="2" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -934,7 +934,7 @@
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet2!A4</f>
-        <v>filmweird31</v>
+        <v>filmweird33</v>
       </c>
       <c r="B4" s="2" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -963,7 +963,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1045,8 +1045,8 @@
   </sheetPr>
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1099,15 +1099,15 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet4!A2</f>
-        <v>tavalinetont31</v>
+        <v>tavalinetont33</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">A3</f>
-        <v>puhtaloom31</v>
+        <v>puhtaloom33</v>
       </c>
       <c r="C2" s="0" t="str">
         <f aca="false">A4</f>
-        <v>filmweird31</v>
+        <v>filmweird33</v>
       </c>
       <c r="D2" s="0" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -1138,15 +1138,15 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet4!C2</f>
-        <v>puhtaloom31</v>
+        <v>puhtaloom33</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">A4</f>
-        <v>filmweird31</v>
+        <v>filmweird33</v>
       </c>
       <c r="C3" s="0" t="str">
         <f aca="false">A2</f>
-        <v>tavalinetont31</v>
+        <v>tavalinetont33</v>
       </c>
       <c r="D3" s="0" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -1177,15 +1177,15 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet4!E2</f>
-        <v>filmweird31</v>
+        <v>filmweird33</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">A2</f>
-        <v>tavalinetont31</v>
+        <v>tavalinetont33</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">A3</f>
-        <v>puhtaloom31</v>
+        <v>puhtaloom33</v>
       </c>
       <c r="D4" s="0" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -1216,10 +1216,8 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" display="selentest@hotmail.com"/>
-    <hyperlink ref="I3" r:id="rId2" display="testimeauto13@mailinator.com"/>
-    <hyperlink ref="J3" r:id="rId3" display="selentest@hotmail.com"/>
-    <hyperlink ref="I4" r:id="rId4" display="vahekonto11@mailinator.com"/>
-    <hyperlink ref="J4" r:id="rId5" display="selentest@hotmail.com"/>
+    <hyperlink ref="J3" r:id="rId2" display="selentest@hotmail.com"/>
+    <hyperlink ref="J4" r:id="rId3" display="selentest@hotmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1239,7 +1237,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
+      <selection pane="topLeft" activeCell="I28" activeCellId="0" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1299,7 +1297,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet5!A2</f>
-        <v>tavalinetont31</v>
+        <v>tavalinetont33</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">Sheet5!D2</f>
@@ -1342,7 +1340,7 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet5!A3</f>
-        <v>puhtaloom31</v>
+        <v>puhtaloom33</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">Sheet5!D3</f>
@@ -1385,7 +1383,7 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet5!A4</f>
-        <v>filmweird31</v>
+        <v>filmweird33</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">Sheet5!D4</f>
@@ -1479,11 +1477,11 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet6!A2</f>
-        <v>tavalinetont31</v>
+        <v>tavalinetont33</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">A3</f>
-        <v>puhtaloom31</v>
+        <v>puhtaloom33</v>
       </c>
       <c r="C2" s="0" t="str">
         <f aca="false">Sheet5!D2</f>
@@ -1502,11 +1500,11 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet6!A3</f>
-        <v>puhtaloom31</v>
+        <v>puhtaloom33</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">A4</f>
-        <v>filmweird31</v>
+        <v>filmweird33</v>
       </c>
       <c r="C3" s="0" t="str">
         <f aca="false">Sheet5!D3</f>
@@ -1525,11 +1523,11 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet6!A4</f>
-        <v>filmweird31</v>
+        <v>filmweird33</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">A2</f>
-        <v>tavalinetont31</v>
+        <v>tavalinetont33</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">Sheet5!D4</f>
@@ -1571,7 +1569,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1612,11 +1610,11 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet5!A2</f>
-        <v>tavalinetont31</v>
+        <v>tavalinetont33</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">A3</f>
-        <v>puhtaloom31</v>
+        <v>puhtaloom33</v>
       </c>
       <c r="C2" s="0" t="str">
         <f aca="false">Sheet5!D2</f>
@@ -1633,17 +1631,17 @@
       </c>
       <c r="G2" s="0" t="str">
         <f aca="false">Sheet5!G2</f>
-        <v>Jalgpalliäss</v>
+        <v>Jalgpalliass</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet5!A3</f>
-        <v>puhtaloom31</v>
+        <v>puhtaloom33</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">A4</f>
-        <v>filmweird31</v>
+        <v>filmweird33</v>
       </c>
       <c r="C3" s="0" t="str">
         <f aca="false">Sheet5!D3</f>
@@ -1666,11 +1664,11 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet5!A4</f>
-        <v>filmweird31</v>
+        <v>filmweird33</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">A2</f>
-        <v>tavalinetont31</v>
+        <v>tavalinetont33</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">Sheet5!D4</f>
@@ -1708,7 +1706,7 @@
   </sheetPr>
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>

</xml_diff>